<commit_message>
[Fixed] No permite ingresar una máquina nueva
</commit_message>
<xml_diff>
--- a/formatos/formato-cargas-fabriles.xlsx
+++ b/formatos/formato-cargas-fabriles.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689C6BA1-52C9-4770-91A3-5AFC8B3B4FA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A76DB0-866A-4FE7-B548-616FADD49556}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Maquinas" sheetId="1" r:id="rId1"/>
+    <sheet name="Carga Fabril" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>

</xml_diff>

<commit_message>
[Fixed] Cambiado insumo por mantenimiento en carga fabril
</commit_message>
<xml_diff>
--- a/formatos/formato-cargas-fabriles.xlsx
+++ b/formatos/formato-cargas-fabriles.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A76DB0-866A-4FE7-B548-616FADD49556}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEE6F0B-AA9C-4555-A78A-0549FC574D3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,10 @@
     <t>Maquina</t>
   </si>
   <si>
-    <t>Insumo</t>
+    <t>Costo</t>
   </si>
   <si>
-    <t>Costo</t>
+    <t>Mantenimiento</t>
   </si>
 </sst>
 </file>
@@ -430,7 +430,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -447,10 +447,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="3"/>
     </row>

</xml_diff>